<commit_message>
Fixed inconsistency in MTT18 - LAB1 sets (correctly)
</commit_message>
<xml_diff>
--- a/inclusion_sets.xlsx
+++ b/inclusion_sets.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/bri-analysis-pp-main/other-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olavobohreramaral/Dropbox/Brazilian Reproducibility Initiative/Análise/bri-analysis-fixing-data-issues(olavo)/other-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F09DED3-4F1A-2047-9A66-ED6125C007D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525525A4-2AE6-E84F-A042-C4599299EDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="16960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2352" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2353" uniqueCount="221">
   <si>
     <t>EXP</t>
   </si>
@@ -1062,7 +1062,7 @@
   <dimension ref="A1:AN193"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="110" workbookViewId="0">
-      <selection activeCell="H66" sqref="H66"/>
+      <selection activeCell="K66" sqref="K66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6160,6 +6160,9 @@
       <c r="J65" t="s">
         <v>103</v>
       </c>
+      <c r="K65" t="s">
+        <v>103</v>
+      </c>
       <c r="L65" t="s">
         <v>103</v>
       </c>

</xml_diff>